<commit_message>
added image and initiated report generation
</commit_message>
<xml_diff>
--- a/Project-Vss.xlsx
+++ b/Project-Vss.xlsx
@@ -663,28 +663,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="131982080"/>
-        <c:axId val="131983616"/>
+        <c:axId val="122660736"/>
+        <c:axId val="122662272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131982080"/>
+        <c:axId val="122660736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131983616"/>
+        <c:crossAx val="122662272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131983616"/>
+        <c:axId val="122662272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,7 +692,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131982080"/>
+        <c:crossAx val="122660736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,7 +729,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1059,7 +1058,7 @@
   <dimension ref="A3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>